<commit_message>
Edited danger log and requirements.
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d1fbe0f7f6eb8fc/Duke_Grad/Spring/ECE568/erss-hwk2-ka266-rm358/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_25898747B466B820DBD8B26A5D648DE9704AF896" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17E5AF53-0769-4A9F-8C2D-C789C92CD676}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Requirements</t>
   </si>
@@ -49,27 +58,18 @@
     <t xml:space="preserve">2.3 Please specify your cache policy (e.g. cache size, replacement policy, when to clean expired reponse) </t>
   </si>
   <si>
-    <t xml:space="preserve">We do not have a max cache size (We had asked professor Brian if we needed to implement a limit for cache and he suggested that was an optional requirement). We clean up the cache when the next request comes to the proxy server. </t>
-  </si>
-  <si>
     <t>3 You should utilize concurrency</t>
   </si>
   <si>
     <t>3.1 Do you spawn a thread/process to handle a request?</t>
   </si>
   <si>
-    <t>Thread</t>
-  </si>
-  <si>
     <t>3.2 Did do you appropriately handle necessary synchronization for your cache (note a simple strategy like "using a mutex to lock to protect the entire cache for every operation" might not be the prefect answer from our perspective)</t>
   </si>
   <si>
     <t>Yes.</t>
   </si>
   <si>
-    <t xml:space="preserve"> We used mutex to lock when operating on common resources (like cache and log file).</t>
-  </si>
-  <si>
     <t>4 You should have a log file to record required information</t>
   </si>
   <si>
@@ -79,15 +79,9 @@
     <t>6.Your code should be robust to external failures. (i.e. What failures did you handle in your code? how do you handle them? You can answer these in your danger log.)</t>
   </si>
   <si>
-    <t>We handle Malformed requests, client/server connection losing connection in between connect call, server sending error response (i.e 404, 501 etc).</t>
-  </si>
-  <si>
     <t>7.You should know the exception guarantees you make (Please specify them (within your danger log).</t>
   </si>
   <si>
-    <t xml:space="preserve">We follow basic guarantee. Boost library has a destructor which closes all sockets. Additionally we ensure that mutex lock is released in case of any exception. Hence no resources are lost. </t>
-  </si>
-  <si>
     <t>8.You should setup docker for submission, per the requirement</t>
   </si>
   <si>
@@ -95,30 +89,38 @@
   </si>
   <si>
     <t>Any extra tests you would like to mention?</t>
+  </si>
+  <si>
+    <t>Yes, threads</t>
+  </si>
+  <si>
+    <t>We do not have a max cache size (We had asked Professor Rogers if we needed to implement a limit for cache and he suggested that was unnecessary to cap the cache size as there are not many HTTP GET requests that can be used). We clean up expired entries in the cache when the next request comes to the proxy server. If there was a cache size limit, this could be easily changed to use LRU when the limit is met.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We used mutexes to lock when operating on common resources (like cache and log file). Each of these used separate mutexes, so that they could both run on different threads at the same time. Additionally, reads from the cache are not always locked on if there will be no data manipulation.</t>
+  </si>
+  <si>
+    <t>We handle many different types of malformed requests, we believe all malformatted responses, client/server connection losing connection in between connect call, server sending error response (i.e 404, 501 etc).</t>
+  </si>
+  <si>
+    <t>We follow basic guarantee. Boost library has a destructor which closes all sockets. Additionally we ensure that mutex lock is released in case of any exception. Allocated heap memory is also deleted. Hence no resources are lost. We attempt to avoid any exception being thrown.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,31 +162,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,24 +189,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -413,7 +469,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -432,7 +488,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -462,7 +518,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -488,7 +544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -514,7 +570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -540,7 +596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -566,7 +622,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -592,7 +648,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -618,7 +674,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -644,7 +700,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -670,7 +726,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -683,9 +739,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -702,7 +764,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -721,7 +783,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -747,7 +809,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -773,7 +835,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +861,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +887,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -851,7 +913,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +939,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +965,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +991,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1017,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,9 +1030,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -984,7 +1052,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1003,7 +1071,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1101,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1127,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1153,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,7 +1179,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1137,7 +1205,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1231,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1257,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1283,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1241,7 +1309,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,46 +1322,55 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="64.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="64.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5"/>
@@ -1301,193 +1378,193 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" ht="16" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" ht="35.65" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="9" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s" s="6">
-        <v>12</v>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s" s="2">
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>15</v>
+    <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" ht="55" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>18</v>
+    <row r="12" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" ht="16" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s" s="2">
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" ht="16" customHeight="1">
-      <c r="A14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s" s="2">
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" ht="43" customHeight="1">
-      <c r="A15" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s" s="2">
+    <row r="15" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s" s="6">
-        <v>22</v>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" ht="35.65" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s" s="2">
+    <row r="16" spans="1:5" ht="54.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s" s="6">
-        <v>24</v>
+      <c r="C16" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" ht="16" customHeight="1">
-      <c r="A17" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s" s="2">
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" ht="16" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s" s="2">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" ht="16" customHeight="1">
-      <c r="A19" t="s" s="3">
-        <v>27</v>
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
@@ -1496,7 +1573,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>